<commit_message>
Preparing the new features
- Sensititvity
- More aggregated data on internvations
</commit_message>
<xml_diff>
--- a/CVX_Kenya/Optimization/optimization.xlsx
+++ b/CVX_Kenya/Optimization/optimization.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\CIVICS_Kenya\CVX_Kenya\Optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DACAAE-103D-4254-B9B8-B0CF99A9ADC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95827FE7-DDA9-4852-BB65-C584E7F88B40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4170" yWindow="-21720" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{E06427C0-47F7-42FD-AC5A-4E340D5BBA6E}"/>
+    <workbookView xWindow="-4170" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{E06427C0-47F7-42FD-AC5A-4E340D5BBA6E}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="0" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">input!#REF!</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">main!$G$12:$G$15</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">main!$G$13:$G$16</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
@@ -34,10 +34,10 @@
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">input!#REF!</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">main!$D$12</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">main!$D$13</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">input!#REF!</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">main!$D$13:$D$15</definedName>
-    <definedName name="solver_lhs3" localSheetId="1" hidden="1">main!$F$12:$F$15</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">main!$D$14:$D$16</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">main!$F$13:$F$16</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
@@ -45,16 +45,16 @@
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">input!#REF!</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">main!$D$19</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">main!$D$20</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">input!#REF!</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">main!$E$12</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">main!$E$13</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">input!#REF!</definedName>
-    <definedName name="solver_rhs2" localSheetId="1" hidden="1">main!$E$13:$E$15</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">main!$E$14:$E$16</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="62">
   <si>
     <t>Scenario</t>
   </si>
@@ -164,15 +164,9 @@
     <t>m3/FU</t>
   </si>
   <si>
-    <t>Saving</t>
-  </si>
-  <si>
     <t>1 M Ksh investment</t>
   </si>
   <si>
-    <t>Pulping_machines_450_109</t>
-  </si>
-  <si>
     <t>Biomass_ongrid</t>
   </si>
   <si>
@@ -240,6 +234,66 @@
   </si>
   <si>
     <t>Payback time</t>
+  </si>
+  <si>
+    <t>PROI</t>
+  </si>
+  <si>
+    <t>PPBT</t>
+  </si>
+  <si>
+    <t>Ecopulpers_450_110</t>
+  </si>
+  <si>
+    <t>Intervetion</t>
+  </si>
+  <si>
+    <t>_450_109</t>
+  </si>
+  <si>
+    <t>Pulping_machines</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>Import Saving</t>
+  </si>
+  <si>
+    <t>Import Investment</t>
+  </si>
+  <si>
+    <t>Water Total Impact</t>
+  </si>
+  <si>
+    <t>Emission Total Impact</t>
+  </si>
+  <si>
+    <t>=Inv+usefullife*Sav</t>
+  </si>
+  <si>
+    <t>Land Total Impact</t>
+  </si>
+  <si>
+    <t>Import Total Impact</t>
+  </si>
+  <si>
+    <t>Workforce Total Impact</t>
+  </si>
+  <si>
+    <t>IMPACT = IMPACT_of_investment + IMPACT_of_operation*USEFUL_LIFE_of_technology</t>
+  </si>
+  <si>
+    <t>Capital Saving</t>
+  </si>
+  <si>
+    <t>ha/FU</t>
+  </si>
+  <si>
+    <t>Capital Investment</t>
+  </si>
+  <si>
+    <t>Capital Total Impact</t>
   </si>
 </sst>
 </file>
@@ -274,18 +328,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -351,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -370,16 +418,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -391,6 +436,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,13 +463,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -502,13 +551,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -584,13 +633,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1361440</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>104140</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>231455</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>48260</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -677,13 +726,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -759,13 +808,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -844,13 +893,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -905,13 +954,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>147320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>35560</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -992,13 +1041,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1074,13 +1123,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1159,13 +1208,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1220,13 +1269,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>147320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>35560</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1307,13 +1356,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1688,175 +1737,292 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7144A5-05C5-46C4-AE10-A8C13BF2BCC8}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.21875" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.77734375" customWidth="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.77734375" customWidth="1"/>
+    <col min="23" max="23" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="20.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="3"/>
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A1" s="16"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="16"/>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="2" t="str">
+        <f>_xlfn.CONCAT(A3,B3)</f>
+        <v>Pulping_machines_450_109</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>28</v>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0</v>
+      </c>
+      <c r="L3" s="5">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>0</v>
+      </c>
+      <c r="R3" s="5">
+        <v>0</v>
+      </c>
+      <c r="S3" s="5">
+        <v>0</v>
+      </c>
+      <c r="T3" s="5">
+        <v>0</v>
+      </c>
+      <c r="U3" s="5">
+        <v>0</v>
+      </c>
+      <c r="V3" s="5"/>
+      <c r="W3" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="X3" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y3" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z3" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA3" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB3" s="17" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0</v>
-      </c>
-      <c r="G3" s="7">
-        <v>0</v>
-      </c>
-      <c r="H3" s="7">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0</v>
-      </c>
-      <c r="K3" s="5">
-        <v>0</v>
-      </c>
-      <c r="L3" s="5">
-        <v>0</v>
-      </c>
-      <c r="M3" s="5">
-        <v>0</v>
-      </c>
-      <c r="N3" s="5">
-        <v>0</v>
-      </c>
-      <c r="O3" s="5">
-        <v>0</v>
-      </c>
-      <c r="P3" s="5">
-        <v>0</v>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="W5" s="17" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1868,20 +2034,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23C3AB91-274C-483E-90B3-FB1858A46850}">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+    <sheetView showGridLines="0" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.44140625" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.44140625" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="7.77734375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="7.77734375" customWidth="1"/>
     <col min="7" max="7" width="10.5546875" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -1896,50 +2062,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="9" t="s">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="9" t="s">
+      <c r="G1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" s="9" t="s">
+      <c r="I1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="K1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="9" t="s">
+      <c r="M1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -1950,47 +2116,47 @@
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="D2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="9" t="s">
+      <c r="F2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="9" t="s">
+      <c r="K2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="9" t="s">
-        <v>22</v>
+      <c r="O2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -1998,397 +2164,450 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="8">
+        <v>18</v>
+      </c>
+      <c r="D3" s="7">
         <v>1</v>
       </c>
-      <c r="E3" s="8">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8">
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
         <v>275.58999999999997</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="12">
         <v>0.95999991986900568</v>
       </c>
-      <c r="H3" s="14">
+      <c r="H3" s="13">
         <v>0.6920654559507966</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="13">
         <v>1.387151911158615</v>
       </c>
-      <c r="J3" s="14">
+      <c r="J3" s="13">
         <v>3.7530802499823039</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="13">
         <v>1.015747927158372E-2</v>
       </c>
-      <c r="L3" s="14">
+      <c r="L3" s="13">
         <v>0.53979996684938669</v>
       </c>
-      <c r="M3" s="14">
+      <c r="M3" s="13">
         <v>9.5046346075832844E-2</v>
       </c>
-      <c r="N3" s="14">
+      <c r="N3" s="13">
         <v>4.2535808170214304E-3</v>
       </c>
-      <c r="O3" s="14">
+      <c r="O3" s="13">
         <v>2.8961654606973748E-3</v>
       </c>
-      <c r="P3" s="14">
+      <c r="P3" s="13">
         <v>1.174013130366802E-3</v>
       </c>
-      <c r="Q3" s="14">
+      <c r="Q3" s="13">
         <v>5.4423870053142309E-2</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="8">
+        <v>18</v>
+      </c>
+      <c r="D4" s="7">
         <v>1</v>
       </c>
-      <c r="E4" s="8">
-        <v>0</v>
-      </c>
-      <c r="F4" s="10">
-        <v>467.04256100921816</v>
-      </c>
-      <c r="G4" s="13">
-        <v>1.000762820243835</v>
-      </c>
-      <c r="H4" s="14">
-        <v>0.20245399978011849</v>
-      </c>
-      <c r="I4" s="14">
-        <v>4.9431615148663166</v>
-      </c>
-      <c r="J4" s="14">
-        <v>4.6191184228518978E-3</v>
-      </c>
-      <c r="K4" s="14">
-        <v>1.443921173631679E-4</v>
-      </c>
-      <c r="L4" s="14">
-        <v>0.12818127009086311</v>
-      </c>
-      <c r="M4" s="14">
-        <v>2.2855708841234449E-2</v>
-      </c>
-      <c r="N4" s="14">
-        <v>7.4838957516476512E-5</v>
-      </c>
-      <c r="O4" s="14">
-        <v>3.578425417799735E-3</v>
-      </c>
-      <c r="P4" s="14">
-        <v>2.8668157756328577E-4</v>
-      </c>
-      <c r="Q4" s="14">
-        <v>3.5829370375722647E-2</v>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <v>275.58999999999997</v>
+      </c>
+      <c r="G4" s="12">
+        <v>0.95999991986900568</v>
+      </c>
+      <c r="H4" s="13">
+        <v>0.6920654559507966</v>
+      </c>
+      <c r="I4" s="13">
+        <v>1.387151911158615</v>
+      </c>
+      <c r="J4" s="13">
+        <v>3.7530802499823039</v>
+      </c>
+      <c r="K4" s="13">
+        <v>1.015747927158372E-2</v>
+      </c>
+      <c r="L4" s="13">
+        <v>0.53979996684938669</v>
+      </c>
+      <c r="M4" s="13">
+        <v>9.5046346075832844E-2</v>
+      </c>
+      <c r="N4" s="13">
+        <v>4.2535808170214304E-3</v>
+      </c>
+      <c r="O4" s="13">
+        <v>2.8961654606973748E-3</v>
+      </c>
+      <c r="P4" s="13">
+        <v>1.174013130366802E-3</v>
+      </c>
+      <c r="Q4" s="13">
+        <v>5.4423870053142309E-2</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="8">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7">
         <v>1</v>
       </c>
-      <c r="E5" s="8">
-        <v>0</v>
-      </c>
-      <c r="F5" s="10">
-        <v>6797.4060000000009</v>
-      </c>
-      <c r="G5" s="13">
-        <v>1.00000015925616</v>
-      </c>
-      <c r="H5" s="14">
-        <v>0.62656182702630758</v>
-      </c>
-      <c r="I5" s="14">
-        <v>1.5960119434696629</v>
-      </c>
-      <c r="J5" s="14">
-        <v>2.3667127534281458E-3</v>
-      </c>
-      <c r="K5" s="14">
-        <v>2.1832435595570132E-3</v>
-      </c>
-      <c r="L5" s="14">
-        <v>0.30856308445800101</v>
-      </c>
-      <c r="M5" s="14">
-        <v>3.137899748980999E-2</v>
-      </c>
-      <c r="N5" s="14">
-        <v>6.1807718884665519E-4</v>
-      </c>
-      <c r="O5" s="14">
-        <v>0.28596529306378221</v>
-      </c>
-      <c r="P5" s="14">
-        <v>1.9501510541886091E-4</v>
-      </c>
-      <c r="Q5" s="14">
-        <v>9.7205753903836012E-2</v>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9">
+        <v>467.04256100921816</v>
+      </c>
+      <c r="G5" s="12">
+        <v>1.000762820243835</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0.20245399978011849</v>
+      </c>
+      <c r="I5" s="13">
+        <v>4.9431615148663166</v>
+      </c>
+      <c r="J5" s="13">
+        <v>4.6191184228518978E-3</v>
+      </c>
+      <c r="K5" s="13">
+        <v>1.443921173631679E-4</v>
+      </c>
+      <c r="L5" s="13">
+        <v>0.12818127009086311</v>
+      </c>
+      <c r="M5" s="13">
+        <v>2.2855708841234449E-2</v>
+      </c>
+      <c r="N5" s="13">
+        <v>7.4838957516476512E-5</v>
+      </c>
+      <c r="O5" s="13">
+        <v>3.578425417799735E-3</v>
+      </c>
+      <c r="P5" s="13">
+        <v>2.8668157756328577E-4</v>
+      </c>
+      <c r="Q5" s="13">
+        <v>3.5829370375722647E-2</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="8">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7">
         <v>1</v>
       </c>
-      <c r="E6" s="8">
-        <v>0</v>
-      </c>
-      <c r="F6" s="10">
-        <f>G7</f>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="9">
+        <v>6797.4060000000009</v>
+      </c>
+      <c r="G6" s="12">
+        <v>1.00000015925616</v>
+      </c>
+      <c r="H6" s="13">
+        <v>0.62656182702630758</v>
+      </c>
+      <c r="I6" s="13">
+        <v>1.5960119434696629</v>
+      </c>
+      <c r="J6" s="13">
+        <v>2.3667127534281458E-3</v>
+      </c>
+      <c r="K6" s="13">
+        <v>2.1832435595570132E-3</v>
+      </c>
+      <c r="L6" s="13">
+        <v>0.30856308445800101</v>
+      </c>
+      <c r="M6" s="13">
+        <v>3.137899748980999E-2</v>
+      </c>
+      <c r="N6" s="13">
+        <v>6.1807718884665519E-4</v>
+      </c>
+      <c r="O6" s="13">
+        <v>0.28596529306378221</v>
+      </c>
+      <c r="P6" s="13">
+        <v>1.9501510541886091E-4</v>
+      </c>
+      <c r="Q6" s="13">
+        <v>9.7205753903836012E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9">
+        <f>G8</f>
         <v>5421.2995378701016</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G7" s="12">
         <v>1</v>
       </c>
-      <c r="H6" s="14">
-        <f>H7/$G$7</f>
+      <c r="H7" s="13">
+        <f>H8/$G$8</f>
         <v>0.60017611682249938</v>
       </c>
-      <c r="I6" s="14">
-        <f>I7</f>
+      <c r="I7" s="13">
+        <f>I8</f>
         <v>1.666177596826546</v>
       </c>
-      <c r="J6" s="14">
-        <f>J7/$G$7</f>
+      <c r="J7" s="13">
+        <f>J8/$G$8</f>
         <v>1.7866706568443057E-3</v>
       </c>
-      <c r="K6" s="14">
-        <f t="shared" ref="K6:Q6" si="0">K7/$G$7</f>
+      <c r="K7" s="13">
+        <f t="shared" ref="K7:Q7" si="0">K8/$G$8</f>
         <v>1.074154253294724E-2</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L7" s="13">
         <f t="shared" si="0"/>
         <v>6.2183632729923683E-4</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M7" s="13">
         <f t="shared" si="0"/>
         <v>1.3960073147690178E-2</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N7" s="13">
         <f t="shared" si="0"/>
         <v>4.4882945517118857E-3</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O7" s="13">
         <f t="shared" si="0"/>
         <v>2.7351872721376896E-3</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P7" s="13">
         <f t="shared" si="0"/>
         <v>1.2205235057779942E-3</v>
       </c>
-      <c r="Q6" s="14">
+      <c r="Q7" s="13">
         <f t="shared" si="0"/>
         <v>5.1284104614026049E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="2" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="8">
-        <f>G7/17</f>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="7">
+        <f>G8/17</f>
         <v>318.8999728158883</v>
       </c>
-      <c r="E7" s="8">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0</v>
-      </c>
-      <c r="G7" s="13">
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="12">
         <v>5421.2995378701016</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H8" s="12">
         <v>3253.734504770488</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I8" s="12">
         <v>1.666177596826546</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J8" s="12">
         <v>9.6860768062761053</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K8" s="12">
         <v>58.233119569878909</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L8" s="12">
         <v>3.3711609938181941</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M8" s="12">
         <v>75.681738104205579</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N8" s="12">
         <v>24.332389179020542</v>
       </c>
-      <c r="O7" s="13">
+      <c r="O8" s="12">
         <v>14.828269494428239</v>
       </c>
-      <c r="P7" s="13">
+      <c r="P8" s="12">
         <v>6.6168235178338364</v>
       </c>
-      <c r="Q7" s="13">
+      <c r="Q8" s="12">
         <v>278.02649264410138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" cm="1">
-        <f t="array" ref="D12">SUM(D3:D6*G12:G15)</f>
-        <v>4999.9999800000005</v>
-      </c>
-      <c r="E12" s="11">
-        <v>5000</v>
-      </c>
-      <c r="F12">
-        <f t="array" ref="F12:F15">-D3:D6*G12:G15+F3:F6</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="12">
-        <v>275.58999999999997</v>
-      </c>
-      <c r="H12" s="2" t="str">
-        <f t="array" ref="H12:H15">B3:B6</f>
-        <v>Ecopulpers</v>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13">
-        <f t="array" ref="D13">SUM(K3:K6*G12:G15)</f>
-        <v>49.999999826402245</v>
-      </c>
-      <c r="E13" s="11">
-        <v>50</v>
+        <v>33</v>
+      </c>
+      <c r="D13" t="e" cm="1">
+        <f t="array" ref="D13">SUM(D3:D7*G13:G16)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E13" s="10">
+        <v>5000</v>
       </c>
       <c r="F13">
-        <v>467.04256100921816</v>
-      </c>
-      <c r="G13" s="12">
-        <v>0</v>
+        <f t="array" ref="F13:F16">-D3:D7*G13:G16+F3:F7</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="11">
+        <v>275.58999999999997</v>
       </c>
       <c r="H13" s="2" t="str">
-        <v>Shading nets</v>
+        <f t="array" ref="H13:H16">B3:B7</f>
+        <v>Ecopulpers_450_110</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" cm="1">
-        <f t="array" ref="D14">SUM(L3:L6*G12:G15)</f>
-        <v>279.3190275651375</v>
-      </c>
-      <c r="E14" s="11">
-        <v>0</v>
+        <v>36</v>
+      </c>
+      <c r="D14" t="e">
+        <f t="array" ref="D14">SUM(K3:K7*G13:G16)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E14" s="10">
+        <v>50</v>
       </c>
       <c r="F14">
-        <v>6382.9836200000009</v>
-      </c>
-      <c r="G14" s="12">
-        <v>414.42237999999998</v>
+        <v>275.58999999999997</v>
+      </c>
+      <c r="G14" s="11">
+        <v>0</v>
       </c>
       <c r="H14" s="2" t="str">
-        <v>Shading trees</v>
+        <v>Ecopulpers</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="e" cm="1">
+        <f t="array" ref="D15">SUM(L3:L7*G13:G16)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>52.620181009218186</v>
+      </c>
+      <c r="G15" s="11">
+        <v>414.42237999999998</v>
+      </c>
+      <c r="H15" s="2" t="str">
+        <v>Shading nets</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15">
-        <f t="array" ref="D15">SUM(J3:J6*G12:G15)</f>
-        <v>1042.9927332009579</v>
-      </c>
-      <c r="E15" s="11">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>1111.3119378701012</v>
-      </c>
-      <c r="G15" s="12">
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="e">
+        <f t="array" ref="D16">SUM(J3:J7*G13:G16)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>2487.4184000000005</v>
+      </c>
+      <c r="G16" s="11">
         <v>4309.9876000000004</v>
       </c>
-      <c r="H15" s="2" t="str">
-        <v>Biomass</v>
+      <c r="H16" s="2" t="str">
+        <v>Shading trees</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
         <v>7</v>
       </c>
-      <c r="D19">
-        <f t="array" ref="D19">SUM(H3:H6*G12:G15)</f>
-        <v>3037.1391838999944</v>
+      <c r="D20" t="e">
+        <f t="array" ref="D20">SUM(H3:H7*G13:G16)</f>
+        <v>#N/A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>